<commit_message>
WIP: pdf content scan test, success searching by keyword in url
</commit_message>
<xml_diff>
--- a/data/output/company_websites_expanded.xlsx
+++ b/data/output/company_websites_expanded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,51 +453,557 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>worldline</t>
+          <t>Segro</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://worldline.com/</t>
+          <t>https://www.segro.com/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.mckinsey.com/~/media/mckinsey/industries/financial%20services/our%20insights/the%202021%20mckinsey%20global%20payments%20report/2021-mckinsey-global-payments-report.pdf</t>
+          <t>https://www.segro.com/media/lgxg3xhc/segro-green-finance-framework.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>worldline</t>
+          <t>Acciona</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://worldline.com/</t>
+          <t>https://www.acciona.com/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://investors.worldline.com/content/dam/investors-worldline-com/assets/documents/universal-registration-document/worldline-2023-financials.pdf</t>
+          <t>https://mediacdn.acciona.com/media/wgigg3am/2021-non-financial-statement-report.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>worldline</t>
+          <t>Acciona</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://worldline.com/</t>
+          <t>https://www.acciona.com/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.frbservices.org/binaries/content/assets/crsocms/financial-services/fednow/general-use-case.pdf</t>
+          <t>https://mediacdn.acciona.com/media/azpc0g0z/consolidated-financial-statements-2019-acciona.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Acciona</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.acciona.com/</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://mediacdn.acciona.com/media/pwud2oip/consolidated-financial-statements.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.pandoragroup.com/</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.pandoragroup.com/-/media/files/investor-relations/emtn-programme/9-sustainability-linked-finance-framework.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/telecomfinance_deal_of_the_year_2015_09_02_2015.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/jun_2019_semestrial_financial_report_en.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/2019_consolidated_financial_statements_1.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/ihs_towers_2015_tmt_finance_awards_03_12_2015.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/wendel_en_h1.2019_financial_statement.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/wp-content/uploads/2022/04/2021-Wendel-extra-financial-information-1.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/fr/file%3A/C%3A/Users/bbeaujean/AppData/Local/Packages/Microsoft.MicrosoftEdge_8wekyb3d8bbwe/TempState/Downloads/IHS_Netherlands_Holdco_B.V._Unaudited_Q2_2020_Financial_Statements%2520%282%29.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/integration_of_esg_targets_into_the_financial_terms_of_syndicated_credit_facility_03.31.2021.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/appointment_chief_financial_officer.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/ihs_towers_wins_two_emea_finance_awards_-_09062015.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/bureau_veritas_cancellation_of_the_dividend_for_the_2019_financial_year.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/2018_consolidated_financial_statements.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/wp-content/uploads/2022/03/2021-Wendel-Consolidated-Financial-Statements.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.tarkett.com/sites/default/files/2021%20Financial%20Results/ENG_Tarkett_H1%202021_Results.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/wp-content/uploads/2022/07/2022-Half-Year-Financial-Report.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/2020_wendel_extra-financial_information.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/consolidated_financial_statements_june_2016_-_published.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/pdfs/presse/2013_07_03_emea_finance_achievement_awards_2__0.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/wp-content/uploads/2021/09/Condensed-consolidated-half-year-financial-statements-June-2021-1.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/201806_-_condensed_consolidated_financial_statements_-_en_0.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/condensed_consolidated_financial_statements_h12017.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.tarkett-group.com/app/uploads/2023/07/27162537/pr-tarkett-2023-half-year-financial-report-available.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/wp-content/uploads/2023/09/half-year-financial-report-september-2023.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Wendel</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/en</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.wendelgroup.com/sites/default/files/2020_consolidated_financial_statements_03182021.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Reply</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/contents/EXPLORING_THE_IMPLEMENTATION_OF_THE_EU_TAXONOMY_FOR_FINANCIAL_INSTITUTIONS.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Reply</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/contents/Avantage-Reply-Sustainable-Finance-EU-Climate-Regulations.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Reply</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/contents/financial-institutions-towards-new-digital-business-models.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Reply</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.reply.com/contents/Sustainable_Finance_Avantage_Reply-1.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>